<commit_message>
Add dance related art and some color stand-in icons
</commit_message>
<xml_diff>
--- a/even-bigger.xlsx
+++ b/even-bigger.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeagles/Documents/Board Games/CUDO Plays/dancefight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335DE01A-6282-804B-92F9-F392950BAA7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22635169-6066-3F48-9C1F-2100AA49B97A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="3460" windowWidth="23780" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25460" yWindow="8640" windowWidth="23780" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,26 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
   <si>
     <t>Title</t>
   </si>
   <si>
-    <t>Attack</t>
-  </si>
-  <si>
-    <t>Defend</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>Art</t>
   </si>
   <si>
-    <t>broadsword.svg</t>
-  </si>
-  <si>
     <t>You may draw 1 card.</t>
   </si>
   <si>
@@ -52,16 +43,7 @@
     <t>Breaks apart against an attack of 5 or more.</t>
   </si>
   <si>
-    <t>daggers.svg</t>
-  </si>
-  <si>
     <t>Cannot be used against Dwarves.</t>
-  </si>
-  <si>
-    <t>battle-axe.svg</t>
-  </si>
-  <si>
-    <t>round-shield.svg</t>
   </si>
   <si>
     <t>2-step</t>
@@ -183,9 +165,6 @@
     </r>
   </si>
   <si>
-    <t>Kind</t>
-  </si>
-  <si>
     <t>If your opponent attacks you may counter +1 Damage</t>
   </si>
   <si>
@@ -233,7 +212,19 @@
     </r>
   </si>
   <si>
-    <t>the first known footage of the move is seen in the 1933 film Wild Boys of the Road</t>
+    <t>Warning: Do not do this move on concrete…for obvious reasons</t>
+  </si>
+  <si>
+    <t>G-Clef</t>
+  </si>
+  <si>
+    <t>Punch-Blast</t>
+  </si>
+  <si>
+    <t>contortionist.svg</t>
+  </si>
+  <si>
+    <t>body-balance.svg</t>
   </si>
 </sst>
 </file>
@@ -657,49 +648,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="116.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>5</v>
@@ -711,18 +700,18 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
@@ -734,16 +723,16 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2000</v>
       </c>
@@ -757,272 +746,272 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
         <v>39</v>
       </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="5" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
         <v>40</v>
       </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="5" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2">
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2">
-        <v>8</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2">
-        <v>8</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
-        <v>8</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2">
-        <v>8</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2">
-        <v>8</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
@@ -1033,18 +1022,18 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
@@ -1056,18 +1045,18 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
@@ -1079,18 +1068,18 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
@@ -1102,18 +1091,18 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
@@ -1125,18 +1114,18 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
@@ -1148,13 +1137,13 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="G21" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Center title art desciption and snark
</commit_message>
<xml_diff>
--- a/even-bigger.xlsx
+++ b/even-bigger.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeagles/Documents/Board Games/CUDO Plays/dancefight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22635169-6066-3F48-9C1F-2100AA49B97A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71BB6E3-C8F6-1848-A735-137009234C83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25460" yWindow="8640" windowWidth="23780" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5020" yWindow="5960" windowWidth="23780" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,30 +107,6 @@
   </si>
   <si>
     <t>Worm</t>
-  </si>
-  <si>
-    <r>
-      <t>also known as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Mini Swipe</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> or Baby Swipe</t>
-    </r>
   </si>
   <si>
     <r>
@@ -168,30 +144,6 @@
     <t>If your opponent attacks you may counter +1 Damage</t>
   </si>
   <si>
-    <r>
-      <t>The move emerged from a similar move called the </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>airtrack</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> while simultaneously travelling in a circular path</t>
-    </r>
-  </si>
-  <si>
     <t>allow b-boys to transition down to the floor and begin performing downrock. Drops may be designed to look flashy painful or both</t>
   </si>
   <si>
@@ -226,12 +178,29 @@
   <si>
     <t>body-balance.svg</t>
   </si>
+  <si>
+    <t>The move emerged from a similar move called the airtrack while simultaneously travelling in a circular path</t>
+  </si>
+  <si>
+    <r>
+      <t>also known as </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Mini Swipe or Baby Swipe</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,13 +225,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -650,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -668,10 +630,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -703,10 +665,10 @@
         <v>3</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -723,13 +685,13 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -749,10 +711,10 @@
         <v>7</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -771,11 +733,11 @@
       <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>32</v>
+      <c r="F5" t="s">
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -795,10 +757,10 @@
         <v>6</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -821,7 +783,7 @@
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -841,10 +803,10 @@
         <v>6</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -864,10 +826,10 @@
         <v>6</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -890,7 +852,7 @@
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -913,7 +875,7 @@
         <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -936,7 +898,7 @@
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -959,7 +921,7 @@
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -982,7 +944,7 @@
         <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1005,7 +967,7 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1028,7 +990,7 @@
         <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1051,7 +1013,7 @@
         <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1074,7 +1036,7 @@
         <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1097,7 +1059,7 @@
         <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1120,7 +1082,7 @@
         <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1140,10 +1102,10 @@
         <v>6</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>